<commit_message>
feat: updated sempyro generation and completed Health-RI v2.0.0 Excel file
</commit_message>
<xml_diff>
--- a/inputs/EUCAIM.xlsx
+++ b/inputs/EUCAIM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderharms/Documents/Projects/Metadata automation/metadata-automation/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46F2AF9-5CB0-B343-87C5-6447678B90A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97914D03-3C78-2648-AC59-6A9D1548AAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="800" windowWidth="36020" windowHeight="20760" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="36000" windowHeight="20300" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1391" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="644">
   <si>
     <t>Property label</t>
   </si>
@@ -1409,9 +1409,6 @@
     <t>https://w3id.org/linkml/</t>
   </si>
   <si>
-    <t>https://www.w3.org/ns/dcat#</t>
-  </si>
-  <si>
     <t>http://purl.org/dc/terms/</t>
   </si>
   <si>
@@ -1431,9 +1428,6 @@
   </si>
   <si>
     <t>https://www.w3.org/ns/dcat/3#</t>
-  </si>
-  <si>
-    <t>http://www.w3.org/2006/vcard/ns#</t>
   </si>
   <si>
     <t>http://xmlns.com/foaf/0.1/</t>
@@ -2182,10 +2176,22 @@
     <t>eucaim</t>
   </si>
   <si>
-    <t>https://cancerimage.eu/ontology/EUCAIM#</t>
-  </si>
-  <si>
     <t>imageSize</t>
+  </si>
+  <si>
+    <t>https://cancerimage.eu/ontology/EUCAIM/</t>
+  </si>
+  <si>
+    <t>vcard:KindShape</t>
+  </si>
+  <si>
+    <t>foaf:AgentShape</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2006/vcard/ns/</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/dcat#</t>
   </si>
 </sst>
 </file>
@@ -3046,11 +3052,21 @@
   <dxfs count="82">
     <dxf>
       <font>
-        <color theme="1"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.59999389629810485"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3066,11 +3082,61 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3096,36 +3162,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
@@ -3146,51 +3182,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3236,11 +3232,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3256,11 +3252,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3276,6 +3272,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -3286,11 +3292,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color theme="1"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5535,7 +5541,7 @@
     <col min="11" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
@@ -6109,42 +6115,42 @@
     <cfRule type="cellIs" dxfId="25" priority="41" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="42" operator="equal">
-      <formula>"Recommended"</formula>
+    <cfRule type="cellIs" dxfId="24" priority="44" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="23" priority="43" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="44" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="22" priority="42" operator="equal">
+      <formula>"Recommended"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:E28">
-    <cfRule type="cellIs" dxfId="21" priority="45" operator="equal">
-      <formula>"Optional"</formula>
+    <cfRule type="cellIs" dxfId="21" priority="48" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="47" operator="equal">
+      <formula>"Mandatory"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="46" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="47" operator="equal">
-      <formula>"Mandatory"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="48" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="18" priority="45" operator="equal">
+      <formula>"Optional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="17" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="54" operator="equal">
+      <formula>"Conditional"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="51" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="52" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="53" operator="equal">
       <formula>"Mandatory"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="54" operator="equal">
-      <formula>"Conditional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F7 E8">
@@ -6153,28 +6159,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F38">
-    <cfRule type="cellIs" dxfId="12" priority="33" operator="equal">
-      <formula>"Not added"</formula>
+    <cfRule type="cellIs" dxfId="12" priority="38" operator="equal">
+      <formula>"Mandatory"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="36" operator="equal">
-      <formula>"Optional"</formula>
+    <cfRule type="cellIs" dxfId="11" priority="39" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="10" priority="37" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="38" operator="equal">
-      <formula>"Mandatory"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="36" operator="equal">
+      <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="39" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="33" operator="equal">
+      <formula>"Not added"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+      <formula>"needs review"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
       <formula>"reviewd"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
-      <formula>"needs review"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H27 H36:H38">
@@ -6186,17 +6192,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1 F1:F7">
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="equal">
-      <formula>"Optional"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="18" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="17" operator="equal">
+      <formula>"Mandatory"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="16" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="17" operator="equal">
-      <formula>"Mandatory"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="18" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="equal">
+      <formula>"Optional"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -6238,8 +6244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1189FF-E617-AB44-8E2D-7CBBF26DD393}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6265,15 +6271,15 @@
         <v>385</v>
       </c>
       <c r="B3" s="146" t="s">
-        <v>396</v>
+        <v>643</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B4" s="146" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -6281,7 +6287,7 @@
         <v>386</v>
       </c>
       <c r="B5" s="146" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -6289,7 +6295,7 @@
         <v>387</v>
       </c>
       <c r="B6" s="146" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -6297,7 +6303,7 @@
         <v>388</v>
       </c>
       <c r="B7" s="146" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -6305,7 +6311,7 @@
         <v>389</v>
       </c>
       <c r="B8" s="146" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -6313,7 +6319,7 @@
         <v>390</v>
       </c>
       <c r="B9" s="146" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -6321,7 +6327,7 @@
         <v>391</v>
       </c>
       <c r="B10" s="146" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -6329,7 +6335,7 @@
         <v>392</v>
       </c>
       <c r="B11" s="146" t="s">
-        <v>404</v>
+        <v>642</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -6337,7 +6343,7 @@
         <v>393</v>
       </c>
       <c r="B12" s="146" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -6345,31 +6351,31 @@
         <v>394</v>
       </c>
       <c r="B13" s="146" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B14" s="146" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B15" s="146" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B16" s="146" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -6377,167 +6383,167 @@
         <v>386</v>
       </c>
       <c r="B17" s="146" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B18" s="146" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B19" s="146" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B20" s="146" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B21" s="146" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B22" s="146" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B23" s="146" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B24" s="146" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B25" s="146" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B26" s="146" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B27" s="146" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B28" s="146" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B29" s="146" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B30" s="146" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B31" s="146" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B32" s="146" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B33" s="146" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B34" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B35" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B36" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>637</v>
+      </c>
+      <c r="B37" s="146" t="s">
         <v>639</v>
-      </c>
-      <c r="B37" s="146" t="s">
-        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -6574,7 +6580,7 @@
     <hyperlink ref="B31" r:id="rId30" xr:uid="{03F5C7D9-B7B1-B849-B1A8-C69532B79FD4}"/>
     <hyperlink ref="B33" r:id="rId31" xr:uid="{35344756-5F64-7340-954C-9EE0831E4A17}"/>
     <hyperlink ref="B32" r:id="rId32" xr:uid="{7C08AFEB-6A23-6043-87B3-B0E59393D460}"/>
-    <hyperlink ref="B37" r:id="rId33" display="https://cancerimage.eu/ontology/EUCAIM" xr:uid="{DB00DF26-D863-1840-A6BA-1C3F1DF6A91E}"/>
+    <hyperlink ref="B37" r:id="rId33" xr:uid="{DB00DF26-D863-1840-A6BA-1C3F1DF6A91E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6585,7 +6591,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6610,53 +6616,62 @@
         <v>383</v>
       </c>
       <c r="D1" s="152" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="B2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F2" s="146"/>
+      <c r="H2" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B3" t="s">
         <v>67</v>
       </c>
       <c r="F3" s="146"/>
+      <c r="H3" t="s">
+        <v>67</v>
+      </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" t="s">
         <v>59</v>
       </c>
       <c r="I4" t="b">
@@ -6736,28 +6751,28 @@
         <v>11</v>
       </c>
       <c r="M1" s="147" t="s">
+        <v>407</v>
+      </c>
+      <c r="N1" s="147" t="s">
+        <v>408</v>
+      </c>
+      <c r="O1" s="147" t="s">
         <v>409</v>
       </c>
-      <c r="N1" s="147" t="s">
+      <c r="P1" s="147" t="s">
         <v>410</v>
       </c>
-      <c r="O1" s="147" t="s">
+      <c r="Q1" s="147" t="s">
+        <v>488</v>
+      </c>
+      <c r="R1" s="147" t="s">
         <v>411</v>
       </c>
-      <c r="P1" s="147" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q1" s="147" t="s">
-        <v>490</v>
-      </c>
-      <c r="R1" s="147" t="s">
-        <v>413</v>
-      </c>
       <c r="S1" s="147" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="T1" s="147" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="U1" s="147"/>
     </row>
@@ -6793,22 +6808,22 @@
       <c r="K2" s="112"/>
       <c r="L2" s="71"/>
       <c r="M2" s="90" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="N2" s="90" t="s">
         <v>379</v>
       </c>
       <c r="O2" s="90" t="s">
+        <v>416</v>
+      </c>
+      <c r="P2" s="90" t="s">
         <v>418</v>
       </c>
-      <c r="P2" s="90" t="s">
-        <v>420</v>
-      </c>
       <c r="R2" s="90" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="U2" s="90" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="96" x14ac:dyDescent="0.2">
@@ -6847,25 +6862,25 @@
       </c>
       <c r="L3" s="83"/>
       <c r="M3" s="90" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="N3" s="90" t="s">
         <v>379</v>
       </c>
       <c r="O3" s="90" t="s">
+        <v>416</v>
+      </c>
+      <c r="P3" s="90" t="s">
         <v>418</v>
       </c>
-      <c r="P3" s="90" t="s">
+      <c r="R3" s="90" t="s">
         <v>420</v>
       </c>
-      <c r="R3" s="90" t="s">
-        <v>422</v>
-      </c>
       <c r="S3" s="90" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="U3" s="90" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="112" x14ac:dyDescent="0.2">
@@ -6904,22 +6919,22 @@
       </c>
       <c r="L4" s="71"/>
       <c r="M4" s="90" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="N4" s="90" t="s">
+        <v>415</v>
+      </c>
+      <c r="O4" s="90" t="s">
         <v>417</v>
       </c>
-      <c r="O4" s="90" t="s">
+      <c r="P4" s="90" t="s">
         <v>419</v>
       </c>
-      <c r="P4" s="90" t="s">
+      <c r="R4" s="90" t="s">
+        <v>507</v>
+      </c>
+      <c r="U4" s="90" t="s">
         <v>421</v>
-      </c>
-      <c r="R4" s="90" t="s">
-        <v>509</v>
-      </c>
-      <c r="U4" s="90" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="48" x14ac:dyDescent="0.2">
@@ -6958,22 +6973,22 @@
       </c>
       <c r="L5" s="83"/>
       <c r="M5" s="90" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="N5" s="90" t="s">
+        <v>415</v>
+      </c>
+      <c r="O5" s="90" t="s">
         <v>417</v>
       </c>
-      <c r="O5" s="90" t="s">
+      <c r="P5" s="90" t="s">
         <v>419</v>
       </c>
-      <c r="P5" s="90" t="s">
+      <c r="R5" s="90" t="s">
+        <v>507</v>
+      </c>
+      <c r="U5" s="90" t="s">
         <v>421</v>
-      </c>
-      <c r="R5" s="90" t="s">
-        <v>509</v>
-      </c>
-      <c r="U5" s="90" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="80" x14ac:dyDescent="0.2">
@@ -7010,22 +7025,22 @@
       <c r="K6" s="112"/>
       <c r="L6" s="71"/>
       <c r="M6" s="90" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="N6" s="90" t="s">
+        <v>415</v>
+      </c>
+      <c r="O6" s="90" t="s">
         <v>417</v>
       </c>
-      <c r="O6" s="90" t="s">
+      <c r="P6" s="90" t="s">
         <v>419</v>
       </c>
-      <c r="P6" s="90" t="s">
+      <c r="R6" s="90" t="s">
+        <v>507</v>
+      </c>
+      <c r="U6" s="90" t="s">
         <v>421</v>
-      </c>
-      <c r="R6" s="90" t="s">
-        <v>509</v>
-      </c>
-      <c r="U6" s="90" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="128" x14ac:dyDescent="0.2">
@@ -7062,22 +7077,22 @@
       <c r="K7" s="112"/>
       <c r="L7" s="83"/>
       <c r="M7" s="90" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="N7" s="90" t="s">
         <v>379</v>
       </c>
       <c r="O7" s="90" t="s">
+        <v>416</v>
+      </c>
+      <c r="P7" s="90" t="s">
         <v>418</v>
       </c>
-      <c r="P7" s="90" t="s">
+      <c r="R7" s="90" t="s">
         <v>420</v>
       </c>
-      <c r="R7" s="90" t="s">
-        <v>422</v>
-      </c>
       <c r="U7" s="90" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="32" x14ac:dyDescent="0.2">
@@ -7116,22 +7131,22 @@
       </c>
       <c r="L8" s="71"/>
       <c r="M8" s="90" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="N8" s="90" t="s">
         <v>379</v>
       </c>
       <c r="O8" s="90" t="s">
+        <v>416</v>
+      </c>
+      <c r="P8" s="90" t="s">
         <v>418</v>
       </c>
-      <c r="P8" s="90" t="s">
-        <v>420</v>
-      </c>
       <c r="R8" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="U8" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="48" x14ac:dyDescent="0.2">
@@ -7170,22 +7185,22 @@
       </c>
       <c r="L9" s="83"/>
       <c r="M9" s="90" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="N9" s="90" t="s">
         <v>379</v>
       </c>
       <c r="O9" s="90" t="s">
+        <v>416</v>
+      </c>
+      <c r="P9" s="90" t="s">
         <v>418</v>
       </c>
-      <c r="P9" s="90" t="s">
+      <c r="R9" s="90" t="s">
         <v>420</v>
       </c>
-      <c r="R9" s="90" t="s">
-        <v>422</v>
-      </c>
       <c r="U9" s="90" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -7930,28 +7945,28 @@
         <v>11</v>
       </c>
       <c r="M1" s="147" t="s">
+        <v>407</v>
+      </c>
+      <c r="N1" s="147" t="s">
+        <v>408</v>
+      </c>
+      <c r="O1" s="147" t="s">
         <v>409</v>
       </c>
-      <c r="N1" s="147" t="s">
+      <c r="P1" s="147" t="s">
         <v>410</v>
       </c>
-      <c r="O1" s="147" t="s">
+      <c r="Q1" s="147" t="s">
+        <v>488</v>
+      </c>
+      <c r="R1" s="147" t="s">
         <v>411</v>
       </c>
-      <c r="P1" s="147" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q1" s="147" t="s">
-        <v>490</v>
-      </c>
-      <c r="R1" s="147" t="s">
-        <v>413</v>
-      </c>
       <c r="S1" s="147" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="T1" s="147" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="U1" s="147"/>
     </row>
@@ -7991,22 +8006,22 @@
       </c>
       <c r="L2" s="90"/>
       <c r="M2" s="58" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="N2" s="58" t="s">
         <v>379</v>
       </c>
       <c r="O2" s="58" t="s">
+        <v>416</v>
+      </c>
+      <c r="P2" s="58" t="s">
         <v>418</v>
       </c>
-      <c r="P2" s="58" t="s">
+      <c r="R2" s="58" t="s">
         <v>420</v>
       </c>
-      <c r="R2" s="58" t="s">
-        <v>422</v>
-      </c>
       <c r="U2" s="58" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="112" x14ac:dyDescent="0.2">
@@ -8045,25 +8060,25 @@
       </c>
       <c r="L3" s="90"/>
       <c r="M3" s="58" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="N3" s="58" t="s">
         <v>379</v>
       </c>
       <c r="O3" s="58" t="s">
+        <v>416</v>
+      </c>
+      <c r="P3" s="58" t="s">
         <v>418</v>
       </c>
-      <c r="P3" s="58" t="s">
-        <v>420</v>
-      </c>
       <c r="R3" s="58" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="S3" s="58" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="U3" s="58" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="32" x14ac:dyDescent="0.2">
@@ -8102,22 +8117,22 @@
       </c>
       <c r="L4" s="90"/>
       <c r="M4" s="58" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="N4" s="58" t="s">
+        <v>415</v>
+      </c>
+      <c r="O4" s="58" t="s">
         <v>417</v>
       </c>
-      <c r="O4" s="58" t="s">
+      <c r="P4" s="58" t="s">
         <v>419</v>
       </c>
-      <c r="P4" s="58" t="s">
-        <v>421</v>
-      </c>
       <c r="R4" s="58" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="U4" s="58" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -8861,22 +8876,22 @@
         <v>11</v>
       </c>
       <c r="M1" s="147" t="s">
+        <v>407</v>
+      </c>
+      <c r="N1" s="147" t="s">
+        <v>408</v>
+      </c>
+      <c r="O1" s="147" t="s">
         <v>409</v>
       </c>
-      <c r="N1" s="147" t="s">
+      <c r="P1" s="147" t="s">
         <v>410</v>
       </c>
-      <c r="O1" s="147" t="s">
+      <c r="Q1" s="147" t="s">
+        <v>488</v>
+      </c>
+      <c r="R1" s="147" t="s">
         <v>411</v>
-      </c>
-      <c r="P1" s="147" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q1" s="147" t="s">
-        <v>490</v>
-      </c>
-      <c r="R1" s="147" t="s">
-        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -8994,28 +9009,28 @@
         <v>11</v>
       </c>
       <c r="M1" s="147" t="s">
+        <v>407</v>
+      </c>
+      <c r="N1" s="147" t="s">
+        <v>408</v>
+      </c>
+      <c r="O1" s="147" t="s">
         <v>409</v>
       </c>
-      <c r="N1" s="147" t="s">
+      <c r="P1" s="147" t="s">
         <v>410</v>
       </c>
-      <c r="O1" s="147" t="s">
+      <c r="Q1" s="147" t="s">
+        <v>488</v>
+      </c>
+      <c r="R1" s="147" t="s">
         <v>411</v>
       </c>
-      <c r="P1" s="147" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q1" s="147" t="s">
-        <v>490</v>
-      </c>
-      <c r="R1" s="147" t="s">
-        <v>413</v>
-      </c>
       <c r="S1" s="147" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="T1" s="147" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="209.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9054,10 +9069,10 @@
       </c>
       <c r="L2" s="71"/>
       <c r="O2" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P2" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="80" x14ac:dyDescent="0.2">
@@ -9080,7 +9095,7 @@
         <v>27</v>
       </c>
       <c r="G3" s="82" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H3" s="81" t="s">
         <v>28</v>
@@ -9096,10 +9111,10 @@
       </c>
       <c r="L3" s="83"/>
       <c r="O3" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P3" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P3" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="73" customFormat="1" ht="144" x14ac:dyDescent="0.2">
@@ -9138,13 +9153,13 @@
       </c>
       <c r="L4" s="71"/>
       <c r="O4" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="P4" s="73" t="s">
         <v>418</v>
       </c>
-      <c r="P4" s="73" t="s">
-        <v>420</v>
-      </c>
       <c r="T4" s="73" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="64" x14ac:dyDescent="0.2">
@@ -9183,10 +9198,10 @@
       </c>
       <c r="L5" s="83"/>
       <c r="O5" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P5" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P5" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -9225,10 +9240,10 @@
       </c>
       <c r="L6" s="71"/>
       <c r="O6" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P6" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P6" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="48" x14ac:dyDescent="0.2">
@@ -9267,10 +9282,10 @@
       </c>
       <c r="L7" s="83"/>
       <c r="O7" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P7" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P7" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9309,13 +9324,13 @@
       </c>
       <c r="L8" s="71"/>
       <c r="O8" s="24" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="64" x14ac:dyDescent="0.2">
@@ -9354,13 +9369,13 @@
       </c>
       <c r="L9" s="83"/>
       <c r="O9" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P9" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="64" x14ac:dyDescent="0.2">
@@ -9399,10 +9414,10 @@
       </c>
       <c r="L10" s="71"/>
       <c r="O10" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P10" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="142" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -9425,7 +9440,7 @@
         <v>27</v>
       </c>
       <c r="G11" s="81" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H11" s="81" t="s">
         <v>28</v>
@@ -9439,10 +9454,10 @@
       <c r="K11" s="84"/>
       <c r="L11" s="83"/>
       <c r="O11" s="142" t="s">
+        <v>416</v>
+      </c>
+      <c r="P11" s="142" t="s">
         <v>418</v>
-      </c>
-      <c r="P11" s="142" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -9481,10 +9496,10 @@
       </c>
       <c r="L12" s="71"/>
       <c r="O12" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P12" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P12" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9523,10 +9538,10 @@
       </c>
       <c r="L13" s="83"/>
       <c r="O13" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P13" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.2">
@@ -9563,10 +9578,10 @@
       <c r="K14" s="106"/>
       <c r="L14" s="151"/>
       <c r="O14" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P14" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P14" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -9589,7 +9604,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="81" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="H15" s="81" t="s">
         <v>28</v>
@@ -9605,10 +9620,10 @@
       </c>
       <c r="L15" s="83"/>
       <c r="O15" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P15" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P15" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="96" x14ac:dyDescent="0.2">
@@ -9647,10 +9662,10 @@
       </c>
       <c r="L16" s="71"/>
       <c r="O16" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P16" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P16" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="96" x14ac:dyDescent="0.2">
@@ -9689,10 +9704,10 @@
       </c>
       <c r="L17" s="83"/>
       <c r="O17" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P17" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -9715,7 +9730,7 @@
         <v>27</v>
       </c>
       <c r="G18" s="78" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="H18" s="78" t="s">
         <v>28</v>
@@ -9729,10 +9744,10 @@
       <c r="K18" s="70"/>
       <c r="L18" s="71"/>
       <c r="O18" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P18" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P18" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="32" x14ac:dyDescent="0.2">
@@ -9771,10 +9786,10 @@
       </c>
       <c r="L19" s="83"/>
       <c r="O19" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P19" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P19" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="48" x14ac:dyDescent="0.2">
@@ -9813,10 +9828,10 @@
       </c>
       <c r="L20" s="71"/>
       <c r="O20" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P20" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="48" x14ac:dyDescent="0.2">
@@ -9855,10 +9870,10 @@
       </c>
       <c r="L21" s="83"/>
       <c r="O21" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P21" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P21" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="128" x14ac:dyDescent="0.2">
@@ -9881,7 +9896,7 @@
         <v>27</v>
       </c>
       <c r="G22" s="78" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="H22" s="78" t="s">
         <v>28</v>
@@ -9897,10 +9912,10 @@
       </c>
       <c r="L22" s="71"/>
       <c r="O22" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P22" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P22" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="32" x14ac:dyDescent="0.2">
@@ -9939,10 +9954,10 @@
       </c>
       <c r="L23" s="83"/>
       <c r="O23" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P23" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="32" x14ac:dyDescent="0.2">
@@ -9981,10 +9996,10 @@
       </c>
       <c r="L24" s="71"/>
       <c r="O24" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P24" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="48" x14ac:dyDescent="0.2">
@@ -10023,13 +10038,13 @@
       </c>
       <c r="L25" s="83"/>
       <c r="O25" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P25" s="24" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="S25" s="24" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -10068,10 +10083,10 @@
       </c>
       <c r="L26" s="71"/>
       <c r="O26" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P26" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -10110,13 +10125,13 @@
       </c>
       <c r="L27" s="83"/>
       <c r="O27" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P27" s="24" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="64" x14ac:dyDescent="0.2">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="75" t="s">
         <v>169</v>
       </c>
@@ -10152,13 +10167,13 @@
       </c>
       <c r="L28" s="71"/>
       <c r="O28" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P28" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q28" s="24" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="64" x14ac:dyDescent="0.2">
@@ -10181,7 +10196,7 @@
         <v>27</v>
       </c>
       <c r="G29" s="81" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="H29" s="81" t="s">
         <v>28</v>
@@ -10197,10 +10212,10 @@
       </c>
       <c r="L29" s="83"/>
       <c r="O29" s="24" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="P29" s="24" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="48" x14ac:dyDescent="0.2">
@@ -10239,10 +10254,10 @@
       </c>
       <c r="L30" s="71"/>
       <c r="O30" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P30" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="112" x14ac:dyDescent="0.2">
@@ -10281,13 +10296,13 @@
       </c>
       <c r="L31" s="83"/>
       <c r="O31" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P31" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q31" s="24" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="48" x14ac:dyDescent="0.2">
@@ -10310,7 +10325,7 @@
         <v>27</v>
       </c>
       <c r="G32" s="78" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H32" s="78" t="s">
         <v>28</v>
@@ -10326,10 +10341,10 @@
       </c>
       <c r="L32" s="71"/>
       <c r="O32" s="24" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="P32" s="24" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="192" x14ac:dyDescent="0.2">
@@ -10366,13 +10381,13 @@
       <c r="K33" s="84"/>
       <c r="L33" s="83"/>
       <c r="O33" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P33" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q33" s="24" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="48" x14ac:dyDescent="0.2">
@@ -10411,13 +10426,13 @@
       </c>
       <c r="L34" s="71"/>
       <c r="O34" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P34" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q34" s="24" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="48" x14ac:dyDescent="0.2">
@@ -10454,13 +10469,13 @@
       <c r="K35" s="84"/>
       <c r="L35" s="83"/>
       <c r="O35" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P35" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q35" s="24" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -10499,13 +10514,13 @@
       </c>
       <c r="L36" s="71"/>
       <c r="O36" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P36" s="24" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="S36" s="24" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -10544,13 +10559,13 @@
       </c>
       <c r="L37" s="83"/>
       <c r="O37" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P37" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q37" s="24" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="64" x14ac:dyDescent="0.2">
@@ -10573,7 +10588,7 @@
         <v>27</v>
       </c>
       <c r="G38" s="78" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H38" s="78" t="s">
         <v>28</v>
@@ -10589,10 +10604,10 @@
       </c>
       <c r="L38" s="71"/>
       <c r="O38" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P38" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P38" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -10615,7 +10630,7 @@
         <v>27</v>
       </c>
       <c r="G39" s="81" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="H39" s="81" t="s">
         <v>28</v>
@@ -10631,10 +10646,10 @@
       </c>
       <c r="L39" s="83"/>
       <c r="O39" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P39" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P39" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="64" x14ac:dyDescent="0.2">
@@ -10673,10 +10688,10 @@
       </c>
       <c r="L40" s="71"/>
       <c r="O40" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P40" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P40" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -10715,16 +10730,16 @@
       </c>
       <c r="L41" s="83"/>
       <c r="O41" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P41" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q41" s="24" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" ht="64" x14ac:dyDescent="0.2">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="75" t="s">
         <v>245</v>
       </c>
@@ -10760,10 +10775,10 @@
       </c>
       <c r="L42" s="71"/>
       <c r="O42" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P42" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -10802,13 +10817,13 @@
       </c>
       <c r="L43" s="83"/>
       <c r="O43" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P43" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P43" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="T43" s="152" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -10847,10 +10862,10 @@
       </c>
       <c r="L44" s="71"/>
       <c r="O44" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P44" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="64" x14ac:dyDescent="0.2">
@@ -10889,10 +10904,10 @@
       </c>
       <c r="L45" s="83"/>
       <c r="O45" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P45" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P45" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -10931,10 +10946,10 @@
       </c>
       <c r="L46" s="71"/>
       <c r="O46" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P46" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -10973,10 +10988,10 @@
       </c>
       <c r="L47" s="83"/>
       <c r="O47" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P47" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10997,7 +11012,7 @@
         <v>27</v>
       </c>
       <c r="G48" s="78" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="H48" s="78" t="s">
         <v>28</v>
@@ -11011,10 +11026,10 @@
       <c r="K48" s="70"/>
       <c r="L48" s="71"/>
       <c r="O48" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P48" s="24" t="s">
         <v>418</v>
-      </c>
-      <c r="P48" s="24" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="49" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.2">
@@ -11134,9 +11149,9 @@
   </sheetPr>
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11202,28 +11217,28 @@
         <v>11</v>
       </c>
       <c r="M1" s="147" t="s">
+        <v>407</v>
+      </c>
+      <c r="N1" s="147" t="s">
+        <v>408</v>
+      </c>
+      <c r="O1" s="147" t="s">
         <v>409</v>
       </c>
-      <c r="N1" s="147" t="s">
+      <c r="P1" s="147" t="s">
         <v>410</v>
       </c>
-      <c r="O1" s="147" t="s">
+      <c r="Q1" s="147" t="s">
+        <v>488</v>
+      </c>
+      <c r="R1" s="147" t="s">
         <v>411</v>
       </c>
-      <c r="P1" s="147" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q1" s="147" t="s">
-        <v>490</v>
-      </c>
-      <c r="R1" s="147" t="s">
-        <v>413</v>
-      </c>
       <c r="S1" s="147" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="T1" s="147" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="209.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11231,14 +11246,14 @@
         <v>257</v>
       </c>
       <c r="B2" s="157" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C2" s="155" t="s">
         <v>259</v>
       </c>
       <c r="D2" s="76"/>
       <c r="E2" s="157" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F2" s="78"/>
       <c r="G2" s="155" t="s">
@@ -11252,16 +11267,16 @@
       <c r="K2" s="70"/>
       <c r="L2" s="71"/>
       <c r="M2" s="155" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P2" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R2" s="90" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="27" x14ac:dyDescent="0.2">
@@ -11269,14 +11284,14 @@
         <v>70</v>
       </c>
       <c r="B3" s="157" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C3" s="155" t="s">
         <v>72</v>
       </c>
       <c r="D3" s="80"/>
       <c r="E3" s="157" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F3" s="81"/>
       <c r="G3" s="155" t="s">
@@ -11290,35 +11305,35 @@
       <c r="K3" s="84"/>
       <c r="L3" s="83"/>
       <c r="M3" s="155" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="O3" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P3" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R3" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="73" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A4" s="153" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B4" s="157" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C4" s="155" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D4" s="86"/>
       <c r="E4" s="157" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F4" s="78"/>
       <c r="G4" s="155" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="H4" s="154" t="s">
         <v>36</v>
@@ -11328,35 +11343,35 @@
       <c r="K4" s="70"/>
       <c r="L4" s="71"/>
       <c r="M4" s="155" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="O4" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P4" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P4" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R4" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="27" x14ac:dyDescent="0.2">
       <c r="A5" s="153" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B5" s="157" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C5" s="155" t="s">
         <v>193</v>
       </c>
       <c r="D5" s="80"/>
       <c r="E5" s="157" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F5" s="81"/>
       <c r="G5" s="155" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="H5" s="154" t="s">
         <v>36</v>
@@ -11366,35 +11381,35 @@
       <c r="K5" s="84"/>
       <c r="L5" s="83"/>
       <c r="M5" s="155" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="O5" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P5" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P5" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R5" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="40" x14ac:dyDescent="0.2">
       <c r="A6" s="153" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="B6" s="157" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C6" s="155" t="s">
         <v>242</v>
       </c>
       <c r="D6" s="86"/>
       <c r="E6" s="157" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F6" s="78"/>
       <c r="G6" s="155" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="H6" s="154" t="s">
         <v>36</v>
@@ -11404,31 +11419,31 @@
       <c r="K6" s="70"/>
       <c r="L6" s="71"/>
       <c r="M6" s="155" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="O6" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P6" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P6" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R6" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="40" x14ac:dyDescent="0.2">
       <c r="A7" s="153" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B7" s="157" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C7" s="155" t="s">
         <v>96</v>
       </c>
       <c r="D7" s="80"/>
       <c r="E7" s="158" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F7" s="81"/>
       <c r="G7" s="155" t="s">
@@ -11442,31 +11457,31 @@
       <c r="K7" s="84"/>
       <c r="L7" s="83"/>
       <c r="M7" s="155" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="O7" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P7" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P7" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R7" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="153" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B8" s="157" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C8" s="155" t="s">
         <v>57</v>
       </c>
       <c r="D8" s="86"/>
       <c r="E8" s="157" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F8" s="78"/>
       <c r="G8" s="155" t="s">
@@ -11480,19 +11495,19 @@
       <c r="K8" s="70"/>
       <c r="L8" s="71"/>
       <c r="M8" s="155" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="O8" s="24" t="s">
-        <v>418</v>
+        <v>473</v>
       </c>
       <c r="P8" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>498</v>
+        <v>640</v>
       </c>
       <c r="R8" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="40" x14ac:dyDescent="0.2">
@@ -11500,14 +11515,14 @@
         <v>186</v>
       </c>
       <c r="B9" s="157" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C9" s="155" t="s">
         <v>188</v>
       </c>
       <c r="D9" s="80"/>
       <c r="E9" s="157" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F9" s="81"/>
       <c r="G9" s="155" t="s">
@@ -11521,24 +11536,24 @@
       <c r="K9" s="84"/>
       <c r="L9" s="83"/>
       <c r="M9" s="155" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="O9" s="24" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="P9" s="24" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q9" s="24" t="s">
-        <v>499</v>
+        <v>641</v>
       </c>
       <c r="R9" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="27" x14ac:dyDescent="0.2">
       <c r="A10" s="153" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B10" s="157" t="s">
         <v>306</v>
@@ -11548,7 +11563,7 @@
       </c>
       <c r="D10" s="86"/>
       <c r="E10" s="157" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F10" s="78"/>
       <c r="G10" s="155" t="s">
@@ -11562,31 +11577,31 @@
       <c r="K10" s="141"/>
       <c r="L10" s="71"/>
       <c r="M10" s="155" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="O10" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P10" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P10" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R10" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="142" customFormat="1" ht="27" x14ac:dyDescent="0.2">
       <c r="A11" s="153" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B11" s="157" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C11" s="155" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="80"/>
       <c r="E11" s="157" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F11" s="81"/>
       <c r="G11" s="155" t="s">
@@ -11600,16 +11615,16 @@
       <c r="K11" s="84"/>
       <c r="L11" s="83"/>
       <c r="M11" s="155" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="O11" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P11" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P11" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R11" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -11617,14 +11632,14 @@
         <v>251</v>
       </c>
       <c r="B12" s="157" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C12" s="155" t="s">
         <v>253</v>
       </c>
       <c r="D12" s="86"/>
       <c r="E12" s="157" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F12" s="78"/>
       <c r="G12" s="155" t="s">
@@ -11638,16 +11653,16 @@
       <c r="K12" s="70"/>
       <c r="L12" s="71"/>
       <c r="M12" s="155" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="O12" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P12" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P12" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R12" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11655,14 +11670,14 @@
         <v>261</v>
       </c>
       <c r="B13" s="157" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C13" s="155" t="s">
         <v>263</v>
       </c>
       <c r="D13" s="94"/>
       <c r="E13" s="157" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F13" s="81"/>
       <c r="G13" s="155" t="s">
@@ -11676,24 +11691,24 @@
       <c r="K13" s="84"/>
       <c r="L13" s="83"/>
       <c r="M13" s="155" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="O13" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P13" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P13" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R13" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="153" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B14" s="157" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C14" s="155" t="s">
         <v>150</v>
@@ -11702,7 +11717,7 @@
       <c r="E14" s="159"/>
       <c r="F14" s="148"/>
       <c r="G14" s="155" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="H14" s="154" t="s">
         <v>337</v>
@@ -11712,24 +11727,24 @@
       <c r="K14" s="106"/>
       <c r="L14" s="151"/>
       <c r="M14" s="155" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="O14" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P14" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R14" s="90" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="153" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B15" s="157" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C15" s="155" t="s">
         <v>145</v>
@@ -11738,7 +11753,7 @@
       <c r="E15" s="159"/>
       <c r="F15" s="81"/>
       <c r="G15" s="155" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="H15" s="154" t="s">
         <v>337</v>
@@ -11748,31 +11763,31 @@
       <c r="K15" s="143"/>
       <c r="L15" s="83"/>
       <c r="M15" s="155" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="O15" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P15" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R15" s="90" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="27" x14ac:dyDescent="0.2">
       <c r="A16" s="153" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B16" s="157" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C16" s="155" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D16" s="86"/>
       <c r="E16" s="157" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F16" s="78"/>
       <c r="G16" s="155" t="s">
@@ -11786,24 +11801,24 @@
       <c r="K16" s="70"/>
       <c r="L16" s="71"/>
       <c r="M16" s="155" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="O16" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P16" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P16" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R16" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="153" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B17" s="157" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C17" s="155" t="s">
         <v>161</v>
@@ -11812,7 +11827,7 @@
       <c r="E17" s="159"/>
       <c r="F17" s="81"/>
       <c r="G17" s="155" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="H17" s="154" t="s">
         <v>337</v>
@@ -11822,24 +11837,24 @@
       <c r="K17" s="84"/>
       <c r="L17" s="83"/>
       <c r="M17" s="155" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="O17" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P17" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R17" s="90" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="153" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B18" s="157" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C18" s="155" t="s">
         <v>166</v>
@@ -11848,7 +11863,7 @@
       <c r="E18" s="159"/>
       <c r="F18" s="78"/>
       <c r="G18" s="155" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="H18" s="154" t="s">
         <v>337</v>
@@ -11858,31 +11873,31 @@
       <c r="K18" s="70"/>
       <c r="L18" s="71"/>
       <c r="M18" s="155" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="O18" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P18" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R18" s="90" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="53" x14ac:dyDescent="0.2">
       <c r="A19" s="153" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B19" s="157" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C19" s="155" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D19" s="80"/>
       <c r="E19" s="157" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F19" s="81"/>
       <c r="G19" s="155" t="s">
@@ -11896,35 +11911,35 @@
       <c r="K19" s="143"/>
       <c r="L19" s="83"/>
       <c r="M19" s="155" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="O19" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P19" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P19" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R19" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="27" x14ac:dyDescent="0.2">
       <c r="A20" s="153" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B20" s="157" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C20" s="155" t="s">
         <v>210</v>
       </c>
       <c r="D20" s="86"/>
       <c r="E20" s="157" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F20" s="78"/>
       <c r="G20" s="155" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="H20" s="154" t="s">
         <v>337</v>
@@ -11934,16 +11949,16 @@
       <c r="K20" s="70"/>
       <c r="L20" s="71"/>
       <c r="M20" s="155" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="O20" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P20" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P20" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R20" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="27" x14ac:dyDescent="0.2">
@@ -11951,7 +11966,7 @@
         <v>137</v>
       </c>
       <c r="B21" s="157" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C21" s="155" t="s">
         <v>139</v>
@@ -11960,7 +11975,7 @@
       <c r="E21" s="159"/>
       <c r="F21" s="81"/>
       <c r="G21" s="155" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="H21" s="154" t="s">
         <v>28</v>
@@ -11970,31 +11985,31 @@
       <c r="K21" s="145"/>
       <c r="L21" s="83"/>
       <c r="M21" s="155" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="O21" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P21" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P21" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R21" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="27" x14ac:dyDescent="0.2">
       <c r="A22" s="153" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B22" s="157" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C22" s="155" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D22" s="76"/>
       <c r="E22" s="157" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F22" s="78"/>
       <c r="G22" s="155" t="s">
@@ -12008,31 +12023,31 @@
       <c r="K22" s="70"/>
       <c r="L22" s="71"/>
       <c r="M22" s="155" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="O22" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P22" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P22" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R22" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="27" x14ac:dyDescent="0.2">
       <c r="A23" s="153" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B23" s="157" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C23" s="155" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D23" s="80"/>
       <c r="E23" s="157" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F23" s="81"/>
       <c r="G23" s="155" t="s">
@@ -12046,31 +12061,31 @@
       <c r="K23" s="84"/>
       <c r="L23" s="83"/>
       <c r="M23" s="155" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="O23" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P23" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P23" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R23" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="27" x14ac:dyDescent="0.2">
       <c r="A24" s="153" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B24" s="157" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C24" s="155" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D24" s="86"/>
       <c r="E24" s="157" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F24" s="78"/>
       <c r="G24" s="155" t="s">
@@ -12084,31 +12099,31 @@
       <c r="K24" s="70"/>
       <c r="L24" s="71"/>
       <c r="M24" s="155" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="O24" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P24" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P24" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R24" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="27" x14ac:dyDescent="0.2">
       <c r="A25" s="153" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B25" s="157" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C25" s="155" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D25" s="80"/>
       <c r="E25" s="157" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="F25" s="81"/>
       <c r="G25" s="155" t="s">
@@ -12122,31 +12137,31 @@
       <c r="K25" s="84"/>
       <c r="L25" s="83"/>
       <c r="M25" s="155" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="O25" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P25" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P25" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R25" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="27" x14ac:dyDescent="0.2">
       <c r="A26" s="153" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B26" s="157" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C26" s="155" t="s">
         <v>331</v>
       </c>
       <c r="D26" s="86"/>
       <c r="E26" s="157" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F26" s="78"/>
       <c r="G26" s="154" t="s">
@@ -12160,31 +12175,31 @@
       <c r="K26" s="70"/>
       <c r="L26" s="71"/>
       <c r="M26" s="155" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="O26" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P26" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P26" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R26" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="27" x14ac:dyDescent="0.2">
       <c r="A27" s="153" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B27" s="157" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C27" s="155" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="80"/>
       <c r="E27" s="157" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F27" s="81"/>
       <c r="G27" s="154" t="s">
@@ -12198,31 +12213,31 @@
       <c r="K27" s="84"/>
       <c r="L27" s="83"/>
       <c r="M27" s="155" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="O27" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P27" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P27" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R27" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="66" x14ac:dyDescent="0.2">
       <c r="A28" s="153" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B28" s="157" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C28" s="155" t="s">
         <v>282</v>
       </c>
       <c r="D28" s="86"/>
       <c r="E28" s="157" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F28" s="78"/>
       <c r="G28" s="154" t="s">
@@ -12236,24 +12251,24 @@
       <c r="K28" s="70"/>
       <c r="L28" s="71"/>
       <c r="M28" s="155" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="O28" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P28" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P28" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R28" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="27" x14ac:dyDescent="0.2">
       <c r="A29" s="153" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B29" s="157" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C29" s="155" t="s">
         <v>332</v>
@@ -12262,7 +12277,7 @@
       <c r="E29" s="159"/>
       <c r="F29" s="81"/>
       <c r="G29" s="154" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H29" s="154" t="s">
         <v>337</v>
@@ -12272,16 +12287,16 @@
       <c r="K29" s="84"/>
       <c r="L29" s="83"/>
       <c r="M29" s="155" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="O29" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P29" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R29" s="90" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="40" x14ac:dyDescent="0.2">
@@ -12289,14 +12304,14 @@
         <v>334</v>
       </c>
       <c r="B30" s="157" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C30" s="155" t="s">
         <v>335</v>
       </c>
       <c r="D30" s="86"/>
       <c r="E30" s="157" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F30" s="78"/>
       <c r="G30" s="154" t="s">
@@ -12310,16 +12325,16 @@
       <c r="K30" s="70"/>
       <c r="L30" s="71"/>
       <c r="M30" s="155" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="O30" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P30" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P30" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R30" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="27" x14ac:dyDescent="0.2">
@@ -12327,18 +12342,18 @@
         <v>224</v>
       </c>
       <c r="B31" s="157" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C31" s="155" t="s">
         <v>226</v>
       </c>
       <c r="D31" s="80"/>
       <c r="E31" s="157" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F31" s="81"/>
       <c r="G31" s="154" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="H31" s="154" t="s">
         <v>28</v>
@@ -12348,16 +12363,16 @@
       <c r="K31" s="84"/>
       <c r="L31" s="83"/>
       <c r="M31" s="155" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="O31" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P31" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P31" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R31" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="53" x14ac:dyDescent="0.2">
@@ -12365,14 +12380,14 @@
         <v>110</v>
       </c>
       <c r="B32" s="157" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C32" s="155" t="s">
         <v>112</v>
       </c>
       <c r="D32" s="76"/>
       <c r="E32" s="157" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="F32" s="78"/>
       <c r="G32" s="154" t="s">
@@ -12386,16 +12401,16 @@
       <c r="K32" s="70"/>
       <c r="L32" s="71"/>
       <c r="M32" s="155" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="O32" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P32" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R32" s="90" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
@@ -12403,14 +12418,14 @@
         <v>267</v>
       </c>
       <c r="B33" s="157" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C33" s="155" t="s">
         <v>269</v>
       </c>
       <c r="D33" s="80"/>
       <c r="E33" s="157" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F33" s="81"/>
       <c r="G33" s="154" t="s">
@@ -12424,31 +12439,31 @@
       <c r="K33" s="84"/>
       <c r="L33" s="83"/>
       <c r="M33" s="155" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="O33" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P33" s="24" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="R33" s="90" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="27" x14ac:dyDescent="0.2">
       <c r="A34" s="153" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B34" s="157" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C34" s="155" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D34" s="86"/>
       <c r="E34" s="157" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F34" s="78"/>
       <c r="G34" s="154" t="s">
@@ -12462,16 +12477,16 @@
       <c r="K34" s="70"/>
       <c r="L34" s="71"/>
       <c r="M34" s="155" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="O34" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="P34" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="P34" s="24" t="s">
-        <v>420</v>
-      </c>
       <c r="R34" s="90" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
@@ -12778,15 +12793,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B1A1CF98C819F4881BB4349588D0C85" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff8ef391852eaca4511043a54bffd4a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfc87205-1831-4b6c-a7b4-76d40079a43e" xmlns:ns3="221af607-abea-4d5e-830c-567dcc03c0ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="201dd8b781da46d5daa37e3355db44fe" ns2:_="" ns3:_="">
     <xsd:import namespace="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
@@ -13029,6 +13035,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
   <ds:schemaRefs>
@@ -13041,14 +13056,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19A23828-4FF7-4569-837D-B1B2C775409F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13065,4 +13072,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>